<commit_message>
feat: OV add solution to 9th tasks in EGE/ and homework/
</commit_message>
<xml_diff>
--- a/EGE/online-olimpiada-OV/9.xlsx
+++ b/EGE/online-olimpiada-OV/9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/EGE/online-olimpiada-OV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\ege\EGE\online-olimpiada-OV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BAAEF0-E271-804F-BE98-021884624603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552635DE-E79E-4C8C-A9CF-D633D9F8FF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист3" sheetId="3" r:id="rId1"/>
@@ -22,6 +22,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Среднее значение меньше, чем значение в 20:00 того дня</t>
+  </si>
+  <si>
+    <t>Ср значение</t>
+  </si>
+  <si>
+    <t>Функция СЧЁТ посчитала, сколько единичек выпало. А где я считал "ИСТИНА" такого уже не будет</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z97"/>
+  <dimension ref="A1:AD97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2:Z92"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -473,8 +487,14 @@
         <f>((Z2A2+B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2+P2+Q2+R2+S2+T2+U2+V2+W2+X2+Y2)/24)&gt;V2</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43191</v>
       </c>
@@ -554,8 +574,23 @@
         <f>(B2+C2+D2+E2+F2+G2+H2+I2+J2+K2+L2+M2+N2+O2+P2+Q2+R2+S2+T2+U2+V2+W2+X2+Y2)/24&lt;V2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA2" s="4">
+        <f>AVERAGE(B2:Y2)</f>
+        <v>18.499999999999996</v>
+      </c>
+      <c r="AB2">
+        <f>IF(AA2&lt;V2,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <f>COUNT(AB2:AB92)</f>
+        <v>91</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43192</v>
       </c>
@@ -635,8 +670,16 @@
         <f t="shared" ref="Z3:Z66" si="0">(B3+C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3+Q3+R3+S3+T3+U3+V3+W3+X3+Y3)/24&lt;V3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA3" s="4">
+        <f t="shared" ref="AA3:AA66" si="1">AVERAGE(B3:Y3)</f>
+        <v>17.945833333333336</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB66" si="2">IF(AA3&lt;V3,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43193</v>
       </c>
@@ -716,8 +759,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA4" s="4">
+        <f t="shared" si="1"/>
+        <v>18.104166666666664</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43194</v>
       </c>
@@ -797,8 +848,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA5" s="4">
+        <f t="shared" si="1"/>
+        <v>17.987500000000001</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43195</v>
       </c>
@@ -878,8 +937,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA6" s="4">
+        <f t="shared" si="1"/>
+        <v>17.729166666666668</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43196</v>
       </c>
@@ -959,8 +1026,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA7" s="4">
+        <f t="shared" si="1"/>
+        <v>18.145833333333332</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43197</v>
       </c>
@@ -1040,8 +1115,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA8" s="4">
+        <f t="shared" si="1"/>
+        <v>17.962500000000002</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43198</v>
       </c>
@@ -1121,8 +1204,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA9" s="4">
+        <f t="shared" si="1"/>
+        <v>18.033333333333331</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43199</v>
       </c>
@@ -1202,8 +1293,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA10" s="4">
+        <f t="shared" si="1"/>
+        <v>18.370833333333334</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43200</v>
       </c>
@@ -1283,8 +1382,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA11" s="4">
+        <f t="shared" si="1"/>
+        <v>18.475000000000001</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43201</v>
       </c>
@@ -1364,8 +1471,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA12" s="4">
+        <f t="shared" si="1"/>
+        <v>17.945833333333333</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43202</v>
       </c>
@@ -1445,8 +1560,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA13" s="4">
+        <f t="shared" si="1"/>
+        <v>18.304166666666664</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43203</v>
       </c>
@@ -1526,8 +1649,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA14" s="4">
+        <f t="shared" si="1"/>
+        <v>17.987500000000001</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43204</v>
       </c>
@@ -1607,8 +1738,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA15" s="4">
+        <f t="shared" si="1"/>
+        <v>18.404166666666665</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43205</v>
       </c>
@@ -1688,8 +1827,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA16" s="4">
+        <f t="shared" si="1"/>
+        <v>18.204166666666669</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43206</v>
       </c>
@@ -1769,8 +1916,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA17" s="4">
+        <f t="shared" si="1"/>
+        <v>18.416666666666668</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43207</v>
       </c>
@@ -1850,8 +2005,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA18" s="4">
+        <f t="shared" si="1"/>
+        <v>17.858333333333338</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43208</v>
       </c>
@@ -1931,8 +2094,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA19" s="4">
+        <f t="shared" si="1"/>
+        <v>17.720833333333331</v>
+      </c>
+      <c r="AB19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43209</v>
       </c>
@@ -2012,8 +2183,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA20" s="4">
+        <f t="shared" si="1"/>
+        <v>17.691666666666663</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43210</v>
       </c>
@@ -2093,8 +2272,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA21" s="4">
+        <f t="shared" si="1"/>
+        <v>18.024999999999995</v>
+      </c>
+      <c r="AB21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43211</v>
       </c>
@@ -2174,8 +2361,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA22" s="4">
+        <f t="shared" si="1"/>
+        <v>18.174999999999997</v>
+      </c>
+      <c r="AB22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43212</v>
       </c>
@@ -2255,8 +2450,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA23" s="4">
+        <f t="shared" si="1"/>
+        <v>18.2</v>
+      </c>
+      <c r="AB23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43213</v>
       </c>
@@ -2336,8 +2539,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA24" s="4">
+        <f t="shared" si="1"/>
+        <v>18.05</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43214</v>
       </c>
@@ -2417,8 +2628,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA25" s="4">
+        <f t="shared" si="1"/>
+        <v>18.087500000000002</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43215</v>
       </c>
@@ -2498,8 +2717,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA26" s="4">
+        <f t="shared" si="1"/>
+        <v>17.975000000000005</v>
+      </c>
+      <c r="AB26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43216</v>
       </c>
@@ -2579,8 +2806,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA27" s="4">
+        <f t="shared" si="1"/>
+        <v>17.962500000000002</v>
+      </c>
+      <c r="AB27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43217</v>
       </c>
@@ -2660,8 +2895,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA28" s="4">
+        <f t="shared" si="1"/>
+        <v>18.012499999999996</v>
+      </c>
+      <c r="AB28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43218</v>
       </c>
@@ -2741,8 +2984,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA29" s="4">
+        <f t="shared" si="1"/>
+        <v>17.683333333333334</v>
+      </c>
+      <c r="AB29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43219</v>
       </c>
@@ -2822,8 +3073,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA30" s="4">
+        <f t="shared" si="1"/>
+        <v>18.312500000000004</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43220</v>
       </c>
@@ -2903,8 +3162,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA31" s="4">
+        <f t="shared" si="1"/>
+        <v>18.033333333333335</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43221</v>
       </c>
@@ -2984,8 +3251,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA32" s="4">
+        <f t="shared" si="1"/>
+        <v>22.729166666666668</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43222</v>
       </c>
@@ -3065,8 +3340,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA33" s="4">
+        <f t="shared" si="1"/>
+        <v>23.245833333333337</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43223</v>
       </c>
@@ -3146,8 +3429,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA34" s="4">
+        <f t="shared" si="1"/>
+        <v>23.537499999999998</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43224</v>
       </c>
@@ -3227,8 +3518,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA35" s="4">
+        <f t="shared" si="1"/>
+        <v>23.3125</v>
+      </c>
+      <c r="AB35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43225</v>
       </c>
@@ -3308,8 +3607,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA36" s="4">
+        <f t="shared" si="1"/>
+        <v>22.841666666666665</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43226</v>
       </c>
@@ -3389,8 +3696,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA37" s="4">
+        <f t="shared" si="1"/>
+        <v>23.191666666666666</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43227</v>
       </c>
@@ -3470,8 +3785,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA38" s="4">
+        <f t="shared" si="1"/>
+        <v>23.075000000000003</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43228</v>
       </c>
@@ -3551,8 +3874,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA39" s="4">
+        <f t="shared" si="1"/>
+        <v>22.979166666666661</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43229</v>
       </c>
@@ -3632,8 +3963,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA40" s="4">
+        <f t="shared" si="1"/>
+        <v>23.120833333333334</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43230</v>
       </c>
@@ -3713,8 +4052,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA41" s="4">
+        <f t="shared" si="1"/>
+        <v>22.679166666666664</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43231</v>
       </c>
@@ -3794,8 +4141,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA42" s="4">
+        <f t="shared" si="1"/>
+        <v>23.054166666666671</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43232</v>
       </c>
@@ -3875,8 +4230,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA43" s="4">
+        <f t="shared" si="1"/>
+        <v>23.308333333333337</v>
+      </c>
+      <c r="AB43">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43233</v>
       </c>
@@ -3956,8 +4319,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA44" s="4">
+        <f t="shared" si="1"/>
+        <v>22.924999999999997</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43234</v>
       </c>
@@ -4037,8 +4408,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA45" s="4">
+        <f t="shared" si="1"/>
+        <v>22.916666666666661</v>
+      </c>
+      <c r="AB45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43235</v>
       </c>
@@ -4118,8 +4497,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA46" s="4">
+        <f t="shared" si="1"/>
+        <v>23.325000000000003</v>
+      </c>
+      <c r="AB46">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43236</v>
       </c>
@@ -4199,8 +4586,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA47" s="4">
+        <f t="shared" si="1"/>
+        <v>23.408333333333335</v>
+      </c>
+      <c r="AB47">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43237</v>
       </c>
@@ -4280,8 +4675,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA48" s="4">
+        <f t="shared" si="1"/>
+        <v>23.175000000000001</v>
+      </c>
+      <c r="AB48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43238</v>
       </c>
@@ -4361,8 +4764,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA49" s="4">
+        <f t="shared" si="1"/>
+        <v>22.708333333333332</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43239</v>
       </c>
@@ -4442,8 +4853,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA50" s="4">
+        <f t="shared" si="1"/>
+        <v>22.808333333333334</v>
+      </c>
+      <c r="AB50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43240</v>
       </c>
@@ -4523,8 +4942,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA51" s="4">
+        <f t="shared" si="1"/>
+        <v>23.029166666666665</v>
+      </c>
+      <c r="AB51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43241</v>
       </c>
@@ -4604,8 +5031,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA52" s="4">
+        <f t="shared" si="1"/>
+        <v>23.137499999999999</v>
+      </c>
+      <c r="AB52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43242</v>
       </c>
@@ -4685,8 +5120,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA53" s="4">
+        <f t="shared" si="1"/>
+        <v>23.125</v>
+      </c>
+      <c r="AB53">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43243</v>
       </c>
@@ -4766,8 +5209,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA54" s="4">
+        <f t="shared" si="1"/>
+        <v>23.429166666666664</v>
+      </c>
+      <c r="AB54">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43244</v>
       </c>
@@ -4847,8 +5298,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA55" s="4">
+        <f t="shared" si="1"/>
+        <v>22.733333333333331</v>
+      </c>
+      <c r="AB55">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43245</v>
       </c>
@@ -4928,8 +5387,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA56" s="4">
+        <f t="shared" si="1"/>
+        <v>22.983333333333331</v>
+      </c>
+      <c r="AB56">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43246</v>
       </c>
@@ -5009,8 +5476,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA57" s="4">
+        <f t="shared" si="1"/>
+        <v>23.316666666666674</v>
+      </c>
+      <c r="AB57">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>43247</v>
       </c>
@@ -5090,8 +5565,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA58" s="4">
+        <f t="shared" si="1"/>
+        <v>22.962500000000002</v>
+      </c>
+      <c r="AB58">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>43248</v>
       </c>
@@ -5171,8 +5654,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA59" s="4">
+        <f t="shared" si="1"/>
+        <v>23.137500000000003</v>
+      </c>
+      <c r="AB59">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>43249</v>
       </c>
@@ -5252,8 +5743,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA60" s="4">
+        <f t="shared" si="1"/>
+        <v>23.029166666666665</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>43250</v>
       </c>
@@ -5333,8 +5832,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA61" s="4">
+        <f t="shared" si="1"/>
+        <v>23.262499999999992</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>43251</v>
       </c>
@@ -5414,8 +5921,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA62" s="4">
+        <f t="shared" si="1"/>
+        <v>23.0625</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>43252</v>
       </c>
@@ -5495,8 +6010,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA63" s="4">
+        <f t="shared" si="1"/>
+        <v>30.241666666666664</v>
+      </c>
+      <c r="AB63">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>43253</v>
       </c>
@@ -5576,8 +6099,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA64" s="4">
+        <f t="shared" si="1"/>
+        <v>30.329166666666666</v>
+      </c>
+      <c r="AB64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>43254</v>
       </c>
@@ -5657,8 +6188,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA65" s="4">
+        <f t="shared" si="1"/>
+        <v>29.866666666666671</v>
+      </c>
+      <c r="AB65">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>43255</v>
       </c>
@@ -5738,8 +6277,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA66" s="4">
+        <f t="shared" si="1"/>
+        <v>30.05</v>
+      </c>
+      <c r="AB66">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>43256</v>
       </c>
@@ -5816,11 +6363,19 @@
         <v>28.3</v>
       </c>
       <c r="Z67" s="6" t="b">
-        <f t="shared" ref="Z67:Z92" si="1">(B67+C67+D67+E67+F67+G67+H67+I67+J67+K67+L67+M67+N67+O67+P67+Q67+R67+S67+T67+U67+V67+W67+X67+Y67)/24&lt;V67</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" ref="Z67:Z92" si="3">(B67+C67+D67+E67+F67+G67+H67+I67+J67+K67+L67+M67+N67+O67+P67+Q67+R67+S67+T67+U67+V67+W67+X67+Y67)/24&lt;V67</f>
+        <v>1</v>
+      </c>
+      <c r="AA67" s="4">
+        <f t="shared" ref="AA67:AA92" si="4">AVERAGE(B67:Y67)</f>
+        <v>30.145833333333325</v>
+      </c>
+      <c r="AB67">
+        <f t="shared" ref="AB67:AB92" si="5">IF(AA67&lt;V67,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>43257</v>
       </c>
@@ -5897,11 +6452,19 @@
         <v>25.7</v>
       </c>
       <c r="Z68" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA68" s="4">
+        <f t="shared" si="4"/>
+        <v>29.987500000000001</v>
+      </c>
+      <c r="AB68">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>43258</v>
       </c>
@@ -5978,11 +6541,19 @@
         <v>27.9</v>
       </c>
       <c r="Z69" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA69" s="4">
+        <f t="shared" si="4"/>
+        <v>30.016666666666666</v>
+      </c>
+      <c r="AB69">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>43259</v>
       </c>
@@ -6059,11 +6630,19 @@
         <v>28.4</v>
       </c>
       <c r="Z70" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA70" s="4">
+        <f t="shared" si="4"/>
+        <v>29.683333333333326</v>
+      </c>
+      <c r="AB70">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>43260</v>
       </c>
@@ -6140,11 +6719,19 @@
         <v>27.7</v>
       </c>
       <c r="Z71" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA71" s="4">
+        <f t="shared" si="4"/>
+        <v>29.929166666666671</v>
+      </c>
+      <c r="AB71">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>43261</v>
       </c>
@@ -6221,11 +6808,19 @@
         <v>28.4</v>
       </c>
       <c r="Z72" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA72" s="4">
+        <f t="shared" si="4"/>
+        <v>30.220833333333331</v>
+      </c>
+      <c r="AB72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>43262</v>
       </c>
@@ -6302,11 +6897,19 @@
         <v>26.6</v>
       </c>
       <c r="Z73" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA73" s="4">
+        <f t="shared" si="4"/>
+        <v>30.120833333333334</v>
+      </c>
+      <c r="AB73">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>43263</v>
       </c>
@@ -6383,11 +6986,19 @@
         <v>28.8</v>
       </c>
       <c r="Z74" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA74" s="4">
+        <f t="shared" si="4"/>
+        <v>30.337499999999995</v>
+      </c>
+      <c r="AB74">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>43264</v>
       </c>
@@ -6464,11 +7075,19 @@
         <v>27.5</v>
       </c>
       <c r="Z75" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA75" s="4">
+        <f t="shared" si="4"/>
+        <v>29.591666666666669</v>
+      </c>
+      <c r="AB75">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>43265</v>
       </c>
@@ -6545,11 +7164,19 @@
         <v>28.7</v>
       </c>
       <c r="Z76" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA76" s="4">
+        <f t="shared" si="4"/>
+        <v>30.187500000000004</v>
+      </c>
+      <c r="AB76">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>43266</v>
       </c>
@@ -6626,11 +7253,19 @@
         <v>25.3</v>
       </c>
       <c r="Z77" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA77" s="4">
+        <f t="shared" si="4"/>
+        <v>30.216666666666665</v>
+      </c>
+      <c r="AB77">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>43267</v>
       </c>
@@ -6707,11 +7342,19 @@
         <v>28.5</v>
       </c>
       <c r="Z78" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA78" s="4">
+        <f t="shared" si="4"/>
+        <v>30.237499999999997</v>
+      </c>
+      <c r="AB78">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>43268</v>
       </c>
@@ -6788,11 +7431,19 @@
         <v>28.5</v>
       </c>
       <c r="Z79" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA79" s="4">
+        <f t="shared" si="4"/>
+        <v>30.029166666666669</v>
+      </c>
+      <c r="AB79">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>43269</v>
       </c>
@@ -6869,11 +7520,19 @@
         <v>26.2</v>
       </c>
       <c r="Z80" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA80" s="4">
+        <f t="shared" si="4"/>
+        <v>30.137500000000006</v>
+      </c>
+      <c r="AB80">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>43270</v>
       </c>
@@ -6950,11 +7609,19 @@
         <v>27.6</v>
       </c>
       <c r="Z81" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA81" s="4">
+        <f t="shared" si="4"/>
+        <v>30.208333333333332</v>
+      </c>
+      <c r="AB81">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>43271</v>
       </c>
@@ -7031,11 +7698,19 @@
         <v>27.2</v>
       </c>
       <c r="Z82" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA82" s="4">
+        <f t="shared" si="4"/>
+        <v>29.908333333333335</v>
+      </c>
+      <c r="AB82">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>43272</v>
       </c>
@@ -7112,11 +7787,19 @@
         <v>25.1</v>
       </c>
       <c r="Z83" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA83" s="4">
+        <f t="shared" si="4"/>
+        <v>29.554166666666664</v>
+      </c>
+      <c r="AB83">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>43273</v>
       </c>
@@ -7193,11 +7876,19 @@
         <v>26.1</v>
       </c>
       <c r="Z84" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA84" s="4">
+        <f t="shared" si="4"/>
+        <v>29.887500000000003</v>
+      </c>
+      <c r="AB84">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>43274</v>
       </c>
@@ -7274,11 +7965,19 @@
         <v>25.9</v>
       </c>
       <c r="Z85" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA85" s="4">
+        <f t="shared" si="4"/>
+        <v>29.862499999999994</v>
+      </c>
+      <c r="AB85">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>43275</v>
       </c>
@@ -7355,11 +8054,19 @@
         <v>25.1</v>
       </c>
       <c r="Z86" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA86" s="4">
+        <f t="shared" si="4"/>
+        <v>29.858333333333331</v>
+      </c>
+      <c r="AB86">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>43276</v>
       </c>
@@ -7436,11 +8143,19 @@
         <v>28.3</v>
       </c>
       <c r="Z87" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA87" s="4">
+        <f t="shared" si="4"/>
+        <v>30.266666666666666</v>
+      </c>
+      <c r="AB87">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>43277</v>
       </c>
@@ -7517,11 +8232,19 @@
         <v>28.9</v>
       </c>
       <c r="Z88" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA88" s="4">
+        <f t="shared" si="4"/>
+        <v>30.087500000000002</v>
+      </c>
+      <c r="AB88">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>43278</v>
       </c>
@@ -7598,11 +8321,19 @@
         <v>26.4</v>
       </c>
       <c r="Z89" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA89" s="4">
+        <f t="shared" si="4"/>
+        <v>29.787499999999998</v>
+      </c>
+      <c r="AB89">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>43279</v>
       </c>
@@ -7679,11 +8410,19 @@
         <v>27.8</v>
       </c>
       <c r="Z90" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA90" s="4">
+        <f t="shared" si="4"/>
+        <v>29.704166666666662</v>
+      </c>
+      <c r="AB90">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>43280</v>
       </c>
@@ -7760,11 +8499,19 @@
         <v>27.7</v>
       </c>
       <c r="Z91" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA91" s="4">
+        <f t="shared" si="4"/>
+        <v>30.233333333333334</v>
+      </c>
+      <c r="AB91">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>43281</v>
       </c>
@@ -7841,17 +8588,25 @@
         <v>25.2</v>
       </c>
       <c r="Z92" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA92" s="4">
+        <f t="shared" si="4"/>
+        <v>30.083333333333329</v>
+      </c>
+      <c r="AB92">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="5"/>
     </row>
   </sheetData>

</xml_diff>